<commit_message>
Add SEO, analytics, about page, deployment scripts, and various improvements
- Add SEO meta tags, Open Graph, structured data to all pages
- Add robots.txt and sitemap.xml
- Add About/Help page with site documentation
- Add analytics page with traffic stats, AI bot detection, 404 tracking
- Add Apache deployment scripts (deploy_apache.sh, update_prod.sh)
- Add map favicon (mapicon.svg)
- Add PB2Y aircraft image
- Add Google Search Console verification route
- Add favicon.ico and favicon.png routes
- Remove View in Report buttons from map
- Fix various bugs and improvements
</commit_message>
<xml_diff>
--- a/patrolReports/Cobia_inferred_positions.xlsx
+++ b/patrolReports/Cobia_inferred_positions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmkna\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A92F45-057A-47D1-B99C-14A1590E72ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFA18A1-DD4F-4197-914A-A6DA8A8803F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C22D5F09-3367-4D77-AF0B-38E1AE4D5A4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>patrol</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Cleared Exmouth Gulf</t>
+  </si>
+  <si>
+    <t>Between Dalupiri &amp; Calayan Islands</t>
+  </si>
+  <si>
+    <t>North of Pratas Island</t>
   </si>
 </sst>
 </file>
@@ -522,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51788274-2E7E-4368-9AAD-4E2C5E9CFD98}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -754,22 +760,22 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>430</v>
+        <v>323</v>
       </c>
       <c r="D9">
         <v>-9</v>
       </c>
       <c r="E9" s="1">
-        <v>16372</v>
+        <v>16364</v>
       </c>
       <c r="F9">
-        <v>0.64800000000000002</v>
+        <v>19.216999999999999</v>
       </c>
       <c r="G9">
-        <v>119.783</v>
+        <v>121.333</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -780,22 +786,22 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>1942</v>
+        <v>400</v>
       </c>
       <c r="D10">
         <v>-9</v>
       </c>
       <c r="E10" s="1">
-        <v>16375</v>
+        <v>16366</v>
       </c>
       <c r="F10">
-        <v>-8.4269999999999996</v>
+        <v>21.012</v>
       </c>
       <c r="G10">
-        <v>115.877</v>
+        <v>116.751</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -803,25 +809,25 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>600</v>
+        <v>430</v>
       </c>
       <c r="D11">
         <v>-9</v>
       </c>
       <c r="E11" s="1">
-        <v>16378</v>
-      </c>
-      <c r="F11" s="3">
-        <v>-22.637</v>
+        <v>16372</v>
+      </c>
+      <c r="F11">
+        <v>0.64800000000000002</v>
       </c>
       <c r="G11">
-        <v>111.34099999999999</v>
+        <v>119.783</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -829,77 +835,77 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>1200</v>
+        <v>1942</v>
       </c>
       <c r="D12">
         <v>-9</v>
       </c>
       <c r="E12" s="1">
-        <v>16381</v>
+        <v>16375</v>
       </c>
       <c r="F12">
-        <v>-32.049999999999997</v>
+        <v>-8.4269999999999996</v>
       </c>
       <c r="G12">
-        <v>115.742</v>
+        <v>115.877</v>
       </c>
       <c r="H12" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>1257</v>
+        <v>600</v>
       </c>
       <c r="D13">
         <v>-9</v>
       </c>
       <c r="E13" s="1">
-        <v>16406</v>
-      </c>
-      <c r="F13">
-        <v>-32.049999999999997</v>
+        <v>16378</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-22.637</v>
       </c>
       <c r="G13">
-        <v>115.742</v>
+        <v>111.34099999999999</v>
       </c>
       <c r="H13" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>2242</v>
+        <v>1200</v>
       </c>
       <c r="D14">
         <v>-9</v>
       </c>
       <c r="E14" s="1">
-        <v>16408</v>
+        <v>16381</v>
       </c>
       <c r="F14">
-        <v>-21.786000000000001</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="G14">
-        <v>111.66500000000001</v>
+        <v>115.742</v>
       </c>
       <c r="H14" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -907,25 +913,25 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>645</v>
+        <v>1257</v>
       </c>
       <c r="D15">
         <v>-9</v>
       </c>
       <c r="E15" s="1">
-        <v>16409</v>
+        <v>16406</v>
       </c>
       <c r="F15">
-        <v>-22.219000000000001</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="G15">
-        <v>114.119</v>
+        <v>115.742</v>
       </c>
       <c r="H15" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -933,25 +939,25 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>1900</v>
+        <v>2242</v>
       </c>
       <c r="D16">
         <v>-9</v>
       </c>
       <c r="E16" s="1">
-        <v>16415</v>
+        <v>16408</v>
       </c>
       <c r="F16">
-        <v>-2.7919999999999998</v>
+        <v>-21.786000000000001</v>
       </c>
       <c r="G16">
-        <v>109.13200000000001</v>
+        <v>111.66500000000001</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -959,25 +965,25 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>14</v>
+        <v>645</v>
       </c>
       <c r="D17">
         <v>-9</v>
       </c>
       <c r="E17" s="1">
-        <v>16417</v>
+        <v>16409</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>-22.219000000000001</v>
       </c>
       <c r="G17">
-        <v>107.84</v>
+        <v>114.119</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -985,25 +991,25 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>258</v>
+        <v>1900</v>
       </c>
       <c r="D18">
         <v>-9</v>
       </c>
       <c r="E18" s="1">
-        <v>16458</v>
+        <v>16415</v>
       </c>
       <c r="F18">
-        <v>-22.219000000000001</v>
+        <v>-2.7919999999999998</v>
       </c>
       <c r="G18">
-        <v>114.119</v>
+        <v>109.13200000000001</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1011,25 +1017,25 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>1915</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>-9</v>
       </c>
       <c r="E19" s="1">
-        <v>16458</v>
+        <v>16417</v>
       </c>
       <c r="F19">
-        <v>-21.771999999999998</v>
+        <v>3</v>
       </c>
       <c r="G19">
-        <v>114.29900000000001</v>
+        <v>107.84</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1037,25 +1043,25 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>130</v>
+        <v>258</v>
       </c>
       <c r="D20">
         <v>-9</v>
       </c>
       <c r="E20" s="1">
-        <v>16459</v>
+        <v>16458</v>
       </c>
       <c r="F20">
-        <v>-21.786999999999999</v>
+        <v>-22.219000000000001</v>
       </c>
       <c r="G20">
-        <v>111.5</v>
+        <v>114.119</v>
       </c>
       <c r="H20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1063,68 +1069,68 @@
         <v>3</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>800</v>
+        <v>1915</v>
       </c>
       <c r="D21">
         <v>-9</v>
       </c>
       <c r="E21" s="1">
-        <v>16461</v>
+        <v>16458</v>
       </c>
       <c r="F21">
-        <v>-32.049999999999997</v>
+        <v>-21.771999999999998</v>
       </c>
       <c r="G21">
-        <v>115.742</v>
+        <v>114.29900000000001</v>
       </c>
       <c r="H21" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>1320</v>
+        <v>130</v>
       </c>
       <c r="D22">
         <v>-9</v>
       </c>
       <c r="E22" s="1">
-        <v>16486</v>
+        <v>16459</v>
       </c>
       <c r="F22">
-        <v>-32.049999999999997</v>
+        <v>-21.786999999999999</v>
       </c>
       <c r="G22">
-        <v>115.742</v>
+        <v>111.5</v>
       </c>
       <c r="H22" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>941</v>
+        <v>800</v>
       </c>
       <c r="D23">
         <v>-9</v>
       </c>
       <c r="E23" s="1">
-        <v>16500</v>
+        <v>16461</v>
       </c>
       <c r="F23">
         <v>-32.049999999999997</v>
@@ -1141,59 +1147,59 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>1200</v>
+        <v>1320</v>
       </c>
       <c r="D24">
         <v>-9</v>
       </c>
       <c r="E24" s="1">
-        <v>16542</v>
+        <v>16486</v>
       </c>
       <c r="F24">
-        <v>14.82</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="G24">
-        <v>120.211</v>
+        <v>115.742</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>1407</v>
+        <v>941</v>
       </c>
       <c r="D25">
         <v>-9</v>
       </c>
       <c r="E25" s="1">
-        <v>16566</v>
+        <v>16500</v>
       </c>
       <c r="F25">
-        <v>14.82</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="G25">
-        <v>120.211</v>
+        <v>115.742</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>1200</v>
@@ -1202,68 +1208,68 @@
         <v>-9</v>
       </c>
       <c r="E26" s="1">
-        <v>16606</v>
+        <v>16542</v>
       </c>
       <c r="F26">
-        <v>-32.049999999999997</v>
+        <v>14.82</v>
       </c>
       <c r="G26">
-        <v>115.742</v>
+        <v>120.211</v>
       </c>
       <c r="H26" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1407</v>
       </c>
       <c r="D27">
         <v>-9</v>
       </c>
       <c r="E27" s="1">
-        <v>16637</v>
+        <v>16566</v>
       </c>
       <c r="F27">
-        <v>-32.049999999999997</v>
+        <v>14.82</v>
       </c>
       <c r="G27">
-        <v>115.742</v>
+        <v>120.211</v>
       </c>
       <c r="H27" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="D28">
         <v>-9</v>
       </c>
       <c r="E28" s="1">
-        <v>16642</v>
+        <v>16606</v>
       </c>
       <c r="F28">
-        <v>-8.8226999999999993</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="G28">
-        <v>114.49</v>
+        <v>115.742</v>
       </c>
       <c r="H28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1271,25 +1277,25 @@
         <v>6</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <v>-9</v>
       </c>
       <c r="E29" s="1">
-        <v>16642</v>
+        <v>16637</v>
       </c>
       <c r="F29">
-        <v>-8.6590000000000007</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="G29">
-        <v>114.22199999999999</v>
+        <v>115.742</v>
       </c>
       <c r="H29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1297,22 +1303,25 @@
         <v>6</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>2010</v>
+        <v>200</v>
       </c>
       <c r="D30">
         <v>-9</v>
       </c>
       <c r="E30" s="1">
-        <v>16643</v>
+        <v>16642</v>
       </c>
       <c r="F30">
-        <v>-7.4180000000000001</v>
+        <v>-8.8226999999999993</v>
       </c>
       <c r="G30">
-        <v>105.357</v>
+        <v>114.49</v>
+      </c>
+      <c r="H30" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1320,25 +1329,25 @@
         <v>6</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>740</v>
+        <v>330</v>
       </c>
       <c r="D31">
         <v>-9</v>
       </c>
       <c r="E31" s="1">
-        <v>16644</v>
+        <v>16642</v>
       </c>
       <c r="F31">
-        <v>-6.4850000000000003</v>
+        <v>-8.6590000000000007</v>
       </c>
       <c r="G31">
-        <v>104.93600000000001</v>
+        <v>114.22199999999999</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1346,25 +1355,22 @@
         <v>6</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>500</v>
+        <v>2010</v>
       </c>
       <c r="D32">
         <v>-9</v>
       </c>
       <c r="E32" s="1">
-        <v>16645</v>
+        <v>16643</v>
       </c>
       <c r="F32">
-        <v>-5.9340000000000002</v>
+        <v>-7.4180000000000001</v>
       </c>
       <c r="G32">
-        <v>105.8</v>
-      </c>
-      <c r="H32" t="s">
-        <v>12</v>
+        <v>105.357</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1372,25 +1378,25 @@
         <v>6</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C33">
-        <v>213</v>
+        <v>740</v>
       </c>
       <c r="D33">
         <v>-9</v>
       </c>
       <c r="E33" s="1">
-        <v>16647</v>
+        <v>16644</v>
       </c>
       <c r="F33">
-        <v>-2.34</v>
+        <v>-6.4850000000000003</v>
       </c>
       <c r="G33">
-        <v>109.05</v>
+        <v>104.93600000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1398,25 +1404,25 @@
         <v>6</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34">
-        <v>810</v>
+        <v>500</v>
       </c>
       <c r="D34">
         <v>-9</v>
       </c>
       <c r="E34" s="1">
-        <v>16648</v>
+        <v>16645</v>
       </c>
       <c r="F34">
-        <v>4.22</v>
+        <v>-5.9340000000000002</v>
       </c>
       <c r="G34">
-        <v>107.22</v>
+        <v>105.8</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1424,25 +1430,25 @@
         <v>6</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C35">
-        <v>1005</v>
+        <v>213</v>
       </c>
       <c r="D35">
         <v>-9</v>
       </c>
       <c r="E35" s="1">
-        <v>16654</v>
+        <v>16647</v>
       </c>
       <c r="F35">
-        <v>14.82</v>
+        <v>-2.34</v>
       </c>
       <c r="G35">
-        <v>120.211</v>
+        <v>109.05</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -1450,55 +1456,59 @@
         <v>6</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C36">
-        <v>2000</v>
+        <v>810</v>
       </c>
       <c r="D36">
         <v>-9</v>
       </c>
       <c r="E36" s="1">
-        <v>16660</v>
+        <v>16648</v>
       </c>
       <c r="F36">
-        <v>21.4</v>
+        <v>4.22</v>
       </c>
       <c r="G36">
-        <v>120.5</v>
-      </c>
-      <c r="H36" s="2"/>
+        <v>107.22</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>6</v>
       </c>
       <c r="B37">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C37">
-        <v>600</v>
+        <v>1005</v>
       </c>
       <c r="D37">
         <v>-9</v>
       </c>
       <c r="E37" s="1">
-        <v>16661</v>
+        <v>16654</v>
       </c>
       <c r="F37">
-        <v>21.4</v>
+        <v>14.82</v>
       </c>
       <c r="G37">
-        <v>123.5</v>
-      </c>
-      <c r="H37" s="2"/>
+        <v>120.211</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>6</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38">
         <v>2000</v>
@@ -1507,65 +1517,61 @@
         <v>-9</v>
       </c>
       <c r="E38" s="1">
-        <v>16661</v>
+        <v>16660</v>
       </c>
       <c r="F38">
         <v>21.4</v>
       </c>
       <c r="G38">
-        <v>123</v>
-      </c>
+        <v>120.5</v>
+      </c>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>6</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C39">
-        <v>2050</v>
+        <v>600</v>
       </c>
       <c r="D39">
         <v>-9</v>
       </c>
       <c r="E39" s="1">
-        <v>16663</v>
+        <v>16661</v>
       </c>
       <c r="F39">
-        <v>22.33</v>
+        <v>21.4</v>
       </c>
       <c r="G39">
-        <v>120.17</v>
-      </c>
-      <c r="H39" t="s">
-        <v>16</v>
-      </c>
+        <v>123.5</v>
+      </c>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>6</v>
       </c>
       <c r="B40">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C40">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="D40">
         <v>-9</v>
       </c>
       <c r="E40" s="1">
-        <v>16667</v>
+        <v>16661</v>
       </c>
       <c r="F40">
-        <v>23.23</v>
+        <v>21.4</v>
       </c>
       <c r="G40">
-        <v>125.49</v>
-      </c>
-      <c r="H40" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1573,24 +1579,76 @@
         <v>6</v>
       </c>
       <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>2050</v>
+      </c>
+      <c r="D41">
+        <v>-9</v>
+      </c>
+      <c r="E41" s="1">
+        <v>16663</v>
+      </c>
+      <c r="F41">
+        <v>22.33</v>
+      </c>
+      <c r="G41">
+        <v>120.17</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>1500</v>
+      </c>
+      <c r="D42">
+        <v>-9</v>
+      </c>
+      <c r="E42" s="1">
+        <v>16667</v>
+      </c>
+      <c r="F42">
+        <v>23.23</v>
+      </c>
+      <c r="G42">
+        <v>125.49</v>
+      </c>
+      <c r="H42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43">
         <v>15</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <v>1200</v>
       </c>
-      <c r="D41">
+      <c r="D43">
         <v>-10</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E43" s="1">
         <v>16671</v>
       </c>
-      <c r="F41">
+      <c r="F43">
         <v>15.222</v>
       </c>
-      <c r="G41">
+      <c r="G43">
         <v>145.72800000000001</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H43" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>